<commit_message>
update class base excel
</commit_message>
<xml_diff>
--- a/1-Excel/class-00-base-excel.xlsx
+++ b/1-Excel/class-00-base-excel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/40cbc61c02823304/Área de Trabalho/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/40cbc61c02823304/Área de Trabalho/Emanuel/Data-Analyst-Course/1-Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="275" documentId="8_{491C1D26-61DC-4852-8EDF-3299C4EF6050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1511F97B-13BE-4E9D-A8EE-522912768C7C}"/>
+  <xr:revisionPtr revIDLastSave="276" documentId="8_{491C1D26-61DC-4852-8EDF-3299C4EF6050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC636BEC-D422-4595-9C42-5B448B541017}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{134D3C76-D541-455F-A7B8-E5D0974EC93B}"/>
   </bookViews>
@@ -170,7 +170,7 @@
     <t>A9</t>
   </si>
   <si>
-    <t>SAMILA</t>
+    <t>emanuel</t>
   </si>
 </sst>
 </file>
@@ -282,7 +282,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -308,9 +308,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -321,14 +318,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -654,7 +647,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E680E24-0911-4BAF-9139-050197B2C114}">
   <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -715,8 +710,7 @@
         <f>IF(D4&gt;$H$9,"ACIMA DA MÉDIA","")</f>
         <v/>
       </c>
-      <c r="F4" s="20"/>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="13" t="s">
         <v>24</v>
       </c>
       <c r="H4" s="3">
@@ -726,7 +720,7 @@
       <c r="O4" t="s">
         <v>35</v>
       </c>
-      <c r="P4" s="25">
+      <c r="P4" s="22">
         <v>45215</v>
       </c>
     </row>
@@ -747,25 +741,24 @@
         <f t="shared" ref="E5:E7" si="0">IF(D5&gt;$H$9,"ACIMA DA MÉDIA","")</f>
         <v/>
       </c>
-      <c r="F5" s="20"/>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="24">
+      <c r="H5" s="21">
         <f>MAX(D:D)</f>
         <v>5000</v>
       </c>
       <c r="K5">
         <v>1</v>
       </c>
-      <c r="L5" s="23">
+      <c r="L5" s="20">
         <f>LARGE(D:D,K5)</f>
         <v>5000</v>
       </c>
       <c r="O5" t="s">
         <v>36</v>
       </c>
-      <c r="P5" s="25">
+      <c r="P5" s="22">
         <v>45216</v>
       </c>
     </row>
@@ -786,25 +779,24 @@
         <f t="shared" si="0"/>
         <v>ACIMA DA MÉDIA</v>
       </c>
-      <c r="F6" s="20"/>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="24">
+      <c r="H6" s="21">
         <f>MIN(D:D)</f>
         <v>2000</v>
       </c>
       <c r="K6">
         <v>2</v>
       </c>
-      <c r="L6" s="23">
+      <c r="L6" s="20">
         <f>LARGE(D:D,K6)</f>
         <v>3000</v>
       </c>
       <c r="O6" t="s">
         <v>37</v>
       </c>
-      <c r="P6" s="25">
+      <c r="P6" s="22">
         <v>45217</v>
       </c>
     </row>
@@ -825,101 +817,99 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F7" s="20"/>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="H7" s="24">
+      <c r="H7" s="21">
         <f>LARGE(D:D,I7)</f>
         <v>5000</v>
       </c>
-      <c r="I7" s="13">
+      <c r="I7" s="12">
         <v>1</v>
       </c>
       <c r="K7">
         <v>3</v>
       </c>
-      <c r="L7" s="23">
+      <c r="L7" s="20">
         <f>LARGE(D:D,K7)</f>
         <v>3000</v>
       </c>
       <c r="O7" t="s">
         <v>38</v>
       </c>
-      <c r="P7" s="25">
+      <c r="P7" s="22">
         <v>45218</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A8" s="18"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="21"/>
-      <c r="G8" s="14" t="s">
+      <c r="A8" s="17"/>
+      <c r="B8" s="6"/>
+      <c r="D8" s="18"/>
+      <c r="G8" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="24">
+      <c r="H8" s="21">
         <f>SMALL(D:D,I8)</f>
         <v>2000</v>
       </c>
-      <c r="I8" s="13">
+      <c r="I8" s="12">
         <v>1</v>
       </c>
       <c r="O8" t="s">
         <v>39</v>
       </c>
-      <c r="P8" s="25">
+      <c r="P8" s="22">
         <v>45219</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="H9" s="24">
+      <c r="H9" s="21">
         <f>AVERAGE(D:D)</f>
         <v>3250</v>
       </c>
       <c r="O9" t="s">
         <v>40</v>
       </c>
-      <c r="P9" s="25">
+      <c r="P9" s="22">
         <v>45220</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="11">
         <v>20</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="13" t="s">
         <v>30</v>
       </c>
       <c r="H10" s="2">
         <f>COUNTA(D:D)</f>
         <v>6</v>
       </c>
-      <c r="I10" s="22">
+      <c r="I10" s="19">
         <f>SUM(D:D)/COUNTA(D4:D7)</f>
         <v>3250</v>
       </c>
       <c r="O10" t="s">
         <v>41</v>
       </c>
-      <c r="P10" s="25">
+      <c r="P10" s="22">
         <v>45221</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="13">
+      <c r="C11" s="12">
         <v>30</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="G11" s="13" t="s">
         <v>31</v>
       </c>
       <c r="H11" s="2">
@@ -932,7 +922,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="D12" s="6"/>
-      <c r="G12" s="14" t="s">
+      <c r="G12" s="13" t="s">
         <v>32</v>
       </c>
       <c r="H12" s="2" t="str">
@@ -950,40 +940,40 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="G13" s="15"/>
+      <c r="G13" s="14"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="16">
+      <c r="B14" s="15">
         <f>C10+C11</f>
         <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="16">
+      <c r="B15" s="15">
         <f>C10-C11</f>
         <v>-10</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="16">
+      <c r="B16" s="15">
         <f>C10*C11</f>
         <v>600</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="16">
+      <c r="B17" s="15">
         <f>C10/C11</f>
         <v>0.66666666666666663</v>
       </c>
@@ -992,10 +982,10 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="16">
+      <c r="B18" s="15">
         <f>C10^C11</f>
         <v>1.073741824E+39</v>
       </c>
@@ -1004,10 +994,10 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="17">
+      <c r="B19" s="16">
         <f>SQRT(C10)</f>
         <v>4.4721359549995796</v>
       </c>
@@ -1016,10 +1006,10 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="16">
+      <c r="B20" s="15">
         <f>(C10+C11)/2</f>
         <v>25</v>
       </c>

</xml_diff>